<commit_message>
6.18 修改 excel 模板
</commit_message>
<xml_diff>
--- a/mySystem/mySystem/xls/Extrusion/A/SOP-MFG-301-R01 吹膜工序生产指令.xlsx
+++ b/mySystem/mySystem/xls/Extrusion/A/SOP-MFG-301-R01 吹膜工序生产指令.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuyang/Documents/workspace/mitcpro/mySystem/mySystem/xls/Extrusion/A/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{99D0DC13-2DC3-3442-A170-F6AAFEA52856}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CE2C9C9F-3A9F-D941-9999-6A0BC6357CB8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="460" windowWidth="27980" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1502,6 +1502,108 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1523,116 +1625,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1978,17 +1978,17 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F5" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="1.83203125" style="5" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="1.5" style="5" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="4" style="5" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="12.83203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="0.1640625" style="5" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="1" style="5" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="0.1640625" style="5" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="12.83203125" style="5" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="10.33203125" style="5" customWidth="1"/>
     <col min="8" max="8" width="20" style="5" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" style="5" customWidth="1"/>
@@ -2022,33 +2022,33 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="33.25" customHeight="1" thickBot="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
     </row>
     <row r="3" spans="1:16" ht="28.75" customHeight="1">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="67"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="53"/>
       <c r="I3" s="49" t="s">
         <v>39</v>
       </c>
@@ -2062,18 +2062,18 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="28.75" customHeight="1" thickBot="1">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="70" t="s">
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="71"/>
-      <c r="H4" s="72"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="58"/>
       <c r="I4" s="46" t="s">
         <v>38</v>
       </c>
@@ -2086,12 +2086,12 @@
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="75"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="61"/>
       <c r="F5" s="7" t="s">
         <v>3</v>
       </c>
@@ -2110,10 +2110,10 @@
       <c r="K5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="76" t="s">
+      <c r="L5" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="77"/>
+      <c r="M5" s="63"/>
       <c r="P5" s="5">
         <f>G8/2500</f>
         <v>0</v>
@@ -2153,12 +2153,12 @@
     </row>
     <row r="8" spans="1:16" s="30" customFormat="1" ht="19.25" customHeight="1" thickBot="1">
       <c r="A8" s="26"/>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="80"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="66"/>
       <c r="F8" s="27"/>
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
@@ -2172,172 +2172,184 @@
       <c r="A9" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="83"/>
-      <c r="F9" s="84" t="s">
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="85"/>
+      <c r="G9" s="71"/>
       <c r="H9" s="32" t="s">
         <v>14</v>
       </c>
       <c r="I9" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="84" t="s">
+      <c r="J9" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="85"/>
-      <c r="L9" s="86" t="s">
+      <c r="K9" s="71"/>
+      <c r="L9" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="87"/>
+      <c r="M9" s="73"/>
     </row>
     <row r="10" spans="1:16" s="30" customFormat="1" ht="24" customHeight="1">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="59"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="77"/>
       <c r="H10" s="34"/>
       <c r="I10" s="35"/>
       <c r="J10" s="36"/>
       <c r="K10" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="88"/>
-      <c r="M10" s="89"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="79"/>
     </row>
     <row r="11" spans="1:16" s="30" customFormat="1" ht="23" customHeight="1">
-      <c r="A11" s="62"/>
-      <c r="B11" s="57" t="s">
+      <c r="A11" s="74"/>
+      <c r="B11" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="59"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="77"/>
       <c r="H11" s="38"/>
       <c r="I11" s="35"/>
       <c r="J11" s="36"/>
       <c r="K11" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="90"/>
-      <c r="M11" s="91"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="81"/>
     </row>
     <row r="12" spans="1:16" s="30" customFormat="1" ht="22" customHeight="1">
-      <c r="A12" s="62"/>
-      <c r="B12" s="60" t="s">
+      <c r="A12" s="74"/>
+      <c r="B12" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="92"/>
       <c r="I12" s="39"/>
       <c r="J12" s="39"/>
       <c r="K12" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="90"/>
-      <c r="M12" s="91"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="81"/>
     </row>
     <row r="13" spans="1:16" s="21" customFormat="1" ht="22" customHeight="1">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="61" t="s">
+      <c r="C13" s="91"/>
+      <c r="D13" s="91"/>
+      <c r="E13" s="91"/>
+      <c r="F13" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
+      <c r="G13" s="92"/>
+      <c r="H13" s="92"/>
       <c r="I13" s="39"/>
       <c r="J13" s="39"/>
       <c r="K13" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="L13" s="90"/>
-      <c r="M13" s="91"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="81"/>
     </row>
     <row r="14" spans="1:16" s="21" customFormat="1" ht="22" customHeight="1">
-      <c r="A14" s="62"/>
-      <c r="B14" s="63" t="s">
+      <c r="A14" s="74"/>
+      <c r="B14" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="73" t="s">
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="93"/>
+      <c r="F14" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
       <c r="I14" s="40"/>
       <c r="J14" s="40"/>
       <c r="K14" s="41"/>
-      <c r="L14" s="92"/>
-      <c r="M14" s="93"/>
+      <c r="L14" s="82"/>
+      <c r="M14" s="83"/>
     </row>
     <row r="15" spans="1:16" ht="19.25" customHeight="1" thickBot="1">
       <c r="A15" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="52"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="85"/>
+      <c r="I15" s="85"/>
+      <c r="J15" s="85"/>
+      <c r="K15" s="85"/>
+      <c r="L15" s="85"/>
+      <c r="M15" s="86"/>
     </row>
     <row r="16" spans="1:16" ht="60.75" customHeight="1" thickBot="1">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="55" t="s">
+      <c r="B16" s="88"/>
+      <c r="C16" s="88"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="88"/>
+      <c r="F16" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="54" t="s">
+      <c r="G16" s="89"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="56"/>
+      <c r="J16" s="88"/>
+      <c r="K16" s="88"/>
+      <c r="L16" s="88"/>
+      <c r="M16" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="I16:M16"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="B14:E14"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:E4"/>
@@ -2354,18 +2366,6 @@
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="L10:M14"/>
-    <mergeCell ref="B15:M15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="I16:M16"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="B14:E14"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>